<commit_message>
Work in progress for XLSX Reader
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/loopXlsxTemplateResult.xlsx
+++ b/src/test/resources/xlsx/loopXlsxTemplateResult.xlsx
@@ -9,39 +9,144 @@
   <sheets>
     <sheet name="Sheet World ABC" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet World ABC'!$A$7:$B$7</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Jebt supports single properties.</t>
   </si>
   <si>
-    <t>Sbet supports property chain, indexed properties, and mapped properties.</t>
-  </si>
-  <si>
-    <t>Empty lines are not a problem.</t>
+    <t>We also support iterating over arrays.</t>
+  </si>
+  <si>
+    <t>A loop should ALWAYS start in the first column, otherwise layout might be messed up during generation. It's fine to have a loop go over multiple lines.</t>
+  </si>
+  <si>
+    <t>Loops will go to next row after every record:</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>You can also have nested loops, but in that case, inner loops cells will be inserted on the same row:</t>
+  </si>
+  <si>
+    <t>Country:</t>
+  </si>
+  <si>
+    <t>List of Friends:</t>
+  </si>
+  <si>
+    <t>Or only one cell per row.</t>
+  </si>
+  <si>
+    <t>Note that cell formatting will be copied over in loops.</t>
+  </si>
+  <si>
+    <t>You can also have loops as text in a cell, but such loops must be opened and closed in the same cell's text.</t>
   </si>
   <si>
     <t>Hello World!</t>
   </si>
   <si>
-    <t>Even with Text formatting: Some bold World! But only the cell font will be preserved. Any text-section specific formatting will be discarded.</t>
-  </si>
-  <si>
-    <t>The postal code of the third customer is 200093.</t>
-  </si>
-  <si>
-    <t>World folks, Let Jebt take on the World</t>
+    <t>You can iterate over multiple cells on a Row. You cannot use Tables, but you can use a Filter as long as the cells with the filters are inserted before any Loop (so they won't move once template is filled)</t>
+  </si>
+  <si>
+    <t>Customer 1</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Customer 2</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Customer 3</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Name: Customer 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alias: bibi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alias: bobo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alias: baba</t>
+  </si>
+  <si>
+    <t>Friend Name: Customer 4</t>
+  </si>
+  <si>
+    <t>Friend Name: Customer 8</t>
+  </si>
+  <si>
+    <t>Name: Customer 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alias: didi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alias: dada</t>
+  </si>
+  <si>
+    <t>Name: Customer 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alias: toto</t>
+  </si>
+  <si>
+    <t>Friend Name: Customer 7</t>
+  </si>
+  <si>
+    <t>Customer: Customer 1</t>
+  </si>
+  <si>
+    <t>Customer: Customer 2</t>
+  </si>
+  <si>
+    <t>Customer: Customer 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the list of aliases for 'Customer 1': </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "bibi"; "bobo"; "baba"; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the list of aliases for 'Customer 2': </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "didi"; "dada"; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the list of aliases for 'Customer 3': </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "toto"; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,16 +171,77 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -83,14 +249,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,50 +647,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F9" s="2" t="s">
-        <v>6</v>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A7:B7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>